<commit_message>
Update to WOS column lookup spreadsheet
</commit_message>
<xml_diff>
--- a/data-raw/WoS Column abbreviations and names.xlsx
+++ b/data-raw/WoS Column abbreviations and names.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/citationsManagement/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/citationManagement/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9028B8EC-3F5C-D24C-9AA3-509F9212103B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0BF340-231C-AC46-B134-EB84D0F59825}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11740" yWindow="860" windowWidth="17960" windowHeight="16940" xr2:uid="{F91BB766-F262-8346-9851-6E3406823EE9}"/>
   </bookViews>
@@ -690,13 +690,13 @@
     <t>authors</t>
   </si>
   <si>
-    <t>author.keywords</t>
-  </si>
-  <si>
     <t>orcid</t>
   </si>
   <si>
     <t>document_type</t>
+  </si>
+  <si>
+    <t>author_keywords</t>
   </si>
 </sst>
 </file>
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698F2563-EF2A-A244-A308-324EB471A0E5}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1270,7 +1270,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1336,7 +1336,7 @@
         <v>43</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1414,7 +1414,7 @@
         <v>57</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>